<commit_message>
updated multiple formation energy
</commit_message>
<xml_diff>
--- a/plotpackage/data/CO2RR.xlsx
+++ b/plotpackage/data/CO2RR.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7050" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="overlayer" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="24">
   <si>
     <t>*</t>
   </si>
@@ -67,6 +67,33 @@
   </si>
   <si>
     <t>*OH</t>
+  </si>
+  <si>
+    <t>*H</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cor. *HOCO  </t>
+  </si>
+  <si>
+    <t>Cor. *CO</t>
+  </si>
+  <si>
+    <t>Cor. CO</t>
+  </si>
+  <si>
+    <t>Cor. *OH</t>
+  </si>
+  <si>
+    <t>Cor. *H</t>
+  </si>
+  <si>
+    <t>distortion energy</t>
+  </si>
+  <si>
+    <t>S</t>
+  </si>
+  <si>
+    <t>D</t>
   </si>
 </sst>
 </file>
@@ -89,12 +116,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -109,9 +142,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -392,15 +431,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="O13" sqref="O13"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -416,8 +455,11 @@
       <c r="F1" s="1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G1" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -436,8 +478,11 @@
       <c r="F2" s="1">
         <v>1.8098528600000368</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G2" s="1">
+        <v>0.50085286000000728</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -456,8 +501,11 @@
       <c r="F3" s="1">
         <v>0.11867331000002324</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G3" s="1">
+        <v>0.63367331000000426</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -476,8 +524,11 @@
       <c r="F4" s="1">
         <v>0.10783329999998514</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G4" s="1">
+        <v>0.33883329999997436</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -496,8 +547,11 @@
       <c r="F5" s="1">
         <v>0.17459011000000046</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G5" s="1">
+        <v>0.54359010999996649</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -516,8 +570,11 @@
       <c r="F6" s="1">
         <v>0.50452117000003582</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G6" s="1">
+        <v>0.72852117000002004</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -536,8 +593,11 @@
       <c r="F7" s="1">
         <v>0.87297696000002034</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G7" s="1">
+        <v>0.81597695999999864</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>10</v>
       </c>
@@ -556,8 +616,11 @@
       <c r="F8" s="1">
         <v>0.96366062999999613</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G8" s="1">
+        <v>0.64666062999998353</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>11</v>
       </c>
@@ -576,8 +639,11 @@
       <c r="F9" s="1">
         <v>1.2506059500000255</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G9" s="1">
+        <v>8.4605950000023356E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>12</v>
       </c>
@@ -585,10 +651,10 @@
         <v>0</v>
       </c>
       <c r="C10">
-        <v>-1.6461211099999744</v>
+        <v>0.58471838999997061</v>
       </c>
       <c r="D10">
-        <v>-0.32179000999998308</v>
+        <v>-0.13328160999999383</v>
       </c>
       <c r="E10">
         <v>0.12300000000000111</v>
@@ -596,25 +662,31 @@
       <c r="F10" s="1">
         <v>-0.322281610000001</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G10" s="1">
+        <v>0.88571839000002051</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>13</v>
       </c>
       <c r="B11">
         <v>0</v>
       </c>
-      <c r="C11">
-        <v>1.0261838700000041</v>
+      <c r="C11" s="2">
+        <v>-1.6461211099999744</v>
       </c>
       <c r="D11">
-        <v>0.3811838699999619</v>
+        <v>-0.32179000999998308</v>
       </c>
       <c r="E11">
         <v>0.12300000000000111</v>
       </c>
       <c r="F11" s="1">
         <v>-1.5327900099999816</v>
+      </c>
+      <c r="G11" s="1">
+        <v>0.16120999000002989</v>
       </c>
     </row>
   </sheetData>
@@ -625,15 +697,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -649,8 +721,11 @@
       <c r="F1" s="1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G1" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -669,8 +744,11 @@
       <c r="F2" s="1">
         <v>1.8098528600000368</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G2" s="1">
+        <v>0.50085286000000728</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -689,8 +767,11 @@
       <c r="F3" s="1">
         <v>1.6399679499999742</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G3" s="1">
+        <v>0.79696795000000797</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -709,8 +790,11 @@
       <c r="F4" s="1">
         <v>0.39921273000004831</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G4" s="1">
+        <v>-3.8787270000002039E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -729,8 +813,11 @@
       <c r="F5" s="1">
         <v>0.35590765000000957</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G5" s="1">
+        <v>0.68490765000001197</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -749,8 +836,11 @@
       <c r="F6" s="1">
         <v>0.60796175999997004</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G6" s="1">
+        <v>0.85096176000001655</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -769,8 +859,11 @@
       <c r="F7" s="1">
         <v>0.80457920999998933</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G7" s="1">
+        <v>0.71857921000002811</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>10</v>
       </c>
@@ -789,8 +882,11 @@
       <c r="F8" s="1">
         <v>1.0591633999999921</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G8" s="1">
+        <v>0.50416340000003679</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>11</v>
       </c>
@@ -809,8 +905,11 @@
       <c r="F9" s="1">
         <v>0.29031816999998128</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G9" s="1">
+        <v>0.47031816999998277</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>12</v>
       </c>
@@ -829,8 +928,11 @@
       <c r="F10" s="1">
         <v>-0.3485783100000468</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G10" s="1">
+        <v>0.81842168999997789</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>13</v>
       </c>
@@ -848,6 +950,9 @@
       </c>
       <c r="F11" s="1">
         <v>-1.9645194700000239</v>
+      </c>
+      <c r="G11" s="1">
+        <v>-0.16751947000000378</v>
       </c>
     </row>
   </sheetData>
@@ -857,15 +962,18 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:O22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="12" max="12" width="8.7265625" style="4"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.35">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -881,8 +989,26 @@
       <c r="F1" s="1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J1" t="s">
+        <v>18</v>
+      </c>
+      <c r="K1" t="s">
+        <v>19</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -901,8 +1027,34 @@
       <c r="F2" s="1">
         <v>1.8098528600000368</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G2" s="1">
+        <v>0.50085286000000728</v>
+      </c>
+      <c r="H2" s="2">
+        <f>C2-C14</f>
+        <v>-3.0639039800000134</v>
+      </c>
+      <c r="I2">
+        <f>D14-D2</f>
+        <v>0.37019343999996401</v>
+      </c>
+      <c r="J2">
+        <f>E2-E14</f>
+        <v>0.123</v>
+      </c>
+      <c r="K2" s="2">
+        <f>F2-F14</f>
+        <v>-7.2975268399999305</v>
+      </c>
+      <c r="L2" s="4">
+        <f>G2-G14</f>
+        <v>0.34289362999999007</v>
+      </c>
+      <c r="O2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -921,9 +1073,35 @@
       <c r="F3" s="1">
         <v>1.5869255800000168</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
+      <c r="G3" s="1">
+        <v>0.76592557999998512</v>
+      </c>
+      <c r="H3">
+        <f t="shared" ref="H3:H11" si="0">C3-C15</f>
+        <v>8.1966039999933571E-2</v>
+      </c>
+      <c r="I3" s="5">
+        <f t="shared" ref="I3:I11" si="1">D15-D3</f>
+        <v>4.2595448900000399</v>
+      </c>
+      <c r="J3">
+        <f t="shared" ref="J3:J11" si="2">E3-E15</f>
+        <v>0.123</v>
+      </c>
+      <c r="K3">
+        <f t="shared" ref="K3:K11" si="3">F3-F15</f>
+        <v>0.81746871000001775</v>
+      </c>
+      <c r="L3" s="4">
+        <f t="shared" ref="L3:L11" si="4">G3-G15</f>
+        <v>0.48539593999998765</v>
+      </c>
+      <c r="O3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B4">
@@ -941,9 +1119,35 @@
       <c r="F4" s="1">
         <v>1.3036249500000316</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
+      <c r="G4" s="1">
+        <v>0.44362495000001267</v>
+      </c>
+      <c r="H4">
+        <f t="shared" si="0"/>
+        <v>6.0624999999774332E-3</v>
+      </c>
+      <c r="I4">
+        <f t="shared" si="1"/>
+        <v>0.75545404000002847</v>
+      </c>
+      <c r="J4">
+        <f t="shared" si="2"/>
+        <v>0.123</v>
+      </c>
+      <c r="K4">
+        <f t="shared" si="3"/>
+        <v>0.38393695000002381</v>
+      </c>
+      <c r="L4" s="4">
+        <f t="shared" si="4"/>
+        <v>0.19018207999999781</v>
+      </c>
+      <c r="O4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A5" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B5">
@@ -961,8 +1165,34 @@
       <c r="F5" s="1">
         <v>0.41203192000000755</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G5" s="1">
+        <v>0.69903191999997993</v>
+      </c>
+      <c r="H5">
+        <f t="shared" si="0"/>
+        <v>-0.10170161000002764</v>
+      </c>
+      <c r="I5">
+        <f t="shared" si="1"/>
+        <v>0.31327278999999564</v>
+      </c>
+      <c r="J5">
+        <f t="shared" si="2"/>
+        <v>0.123</v>
+      </c>
+      <c r="K5">
+        <f t="shared" si="3"/>
+        <v>-6.0994279999984968E-2</v>
+      </c>
+      <c r="L5" s="4">
+        <f t="shared" si="4"/>
+        <v>0.69550219999996266</v>
+      </c>
+      <c r="O5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -981,9 +1211,35 @@
       <c r="F6" s="1">
         <v>0.60696899999999587</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
+      <c r="G6" s="1">
+        <v>0.76996900000000146</v>
+      </c>
+      <c r="H6">
+        <f t="shared" si="0"/>
+        <v>0.15017116000000641</v>
+      </c>
+      <c r="I6">
+        <f t="shared" si="1"/>
+        <v>7.4675719999969914E-2</v>
+      </c>
+      <c r="J6">
+        <f t="shared" si="2"/>
+        <v>0.123</v>
+      </c>
+      <c r="K6">
+        <f t="shared" si="3"/>
+        <v>-0.21946666999997078</v>
+      </c>
+      <c r="L6" s="4">
+        <f t="shared" si="4"/>
+        <v>0.60617510999997926</v>
+      </c>
+      <c r="O6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A7" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B7">
@@ -1001,9 +1257,35 @@
       <c r="F7" s="1">
         <v>0.80585626999999604</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
+      <c r="G7" s="1">
+        <v>0.94685627000001027</v>
+      </c>
+      <c r="H7">
+        <f t="shared" si="0"/>
+        <v>0.53262588000000477</v>
+      </c>
+      <c r="I7" s="2">
+        <f t="shared" si="1"/>
+        <v>12.404627159999972</v>
+      </c>
+      <c r="J7">
+        <f t="shared" si="2"/>
+        <v>0.123</v>
+      </c>
+      <c r="K7">
+        <f t="shared" si="3"/>
+        <v>3.1372239999999607E-2</v>
+      </c>
+      <c r="L7" s="4">
+        <f t="shared" si="4"/>
+        <v>0.73375338000005108</v>
+      </c>
+      <c r="O7" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A8" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B8">
@@ -1021,8 +1303,34 @@
       <c r="F8" s="1">
         <v>0.9946521099999508</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G8" s="1">
+        <v>0.62565210999997412</v>
+      </c>
+      <c r="H8">
+        <f t="shared" si="0"/>
+        <v>0.6519396699999831</v>
+      </c>
+      <c r="I8">
+        <f t="shared" si="1"/>
+        <v>1.0468790800000072</v>
+      </c>
+      <c r="J8">
+        <f t="shared" si="2"/>
+        <v>0.123</v>
+      </c>
+      <c r="K8">
+        <f t="shared" si="3"/>
+        <v>0.63191108999996359</v>
+      </c>
+      <c r="L8" s="4">
+        <f t="shared" si="4"/>
+        <v>0.39718764000002516</v>
+      </c>
+      <c r="O8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>11</v>
       </c>
@@ -1041,8 +1349,34 @@
       <c r="F9" s="1">
         <v>1.9442673999999478</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G9" s="1">
+        <v>0.42926739999995611</v>
+      </c>
+      <c r="H9">
+        <f t="shared" si="0"/>
+        <v>-0.1992254600000436</v>
+      </c>
+      <c r="I9">
+        <f t="shared" si="1"/>
+        <v>-2.2485269999936719E-2</v>
+      </c>
+      <c r="J9">
+        <f t="shared" si="2"/>
+        <v>0.123</v>
+      </c>
+      <c r="K9">
+        <f t="shared" si="3"/>
+        <v>1.128989369999946</v>
+      </c>
+      <c r="L9" s="4">
+        <f t="shared" si="4"/>
+        <v>0.29147088999996917</v>
+      </c>
+      <c r="O9" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>12</v>
       </c>
@@ -1061,8 +1395,34 @@
       <c r="F10" s="1">
         <v>-0.21158410000003514</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G10" s="1">
+        <v>0.77941590000000183</v>
+      </c>
+      <c r="H10" s="2">
+        <f t="shared" si="0"/>
+        <v>-1.1729743400000601</v>
+      </c>
+      <c r="I10">
+        <f t="shared" si="1"/>
+        <v>0.1933609300000505</v>
+      </c>
+      <c r="J10">
+        <f t="shared" si="2"/>
+        <v>0.123</v>
+      </c>
+      <c r="K10" s="2">
+        <f t="shared" si="3"/>
+        <v>-1.3210697300000298</v>
+      </c>
+      <c r="L10" s="4">
+        <f t="shared" si="4"/>
+        <v>0.24522582000002835</v>
+      </c>
+      <c r="O10" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>13</v>
       </c>
@@ -1081,23 +1441,215 @@
       <c r="F11" s="1">
         <v>-0.84702376000000967</v>
       </c>
+      <c r="G11" s="1">
+        <v>0.73697623999998818</v>
+      </c>
+      <c r="H11">
+        <f t="shared" si="0"/>
+        <v>0.2269762399999351</v>
+      </c>
+      <c r="I11">
+        <f t="shared" si="1"/>
+        <v>0.13602376000001115</v>
+      </c>
+      <c r="J11">
+        <f t="shared" si="2"/>
+        <v>0.123</v>
+      </c>
+      <c r="K11">
+        <f t="shared" si="3"/>
+        <v>-0.84702376000000967</v>
+      </c>
+      <c r="L11" s="4">
+        <f t="shared" si="4"/>
+        <v>0.73697623999998818</v>
+      </c>
+      <c r="O11" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="C13" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="3"/>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="C14">
+        <v>3.8827568400000132</v>
+      </c>
+      <c r="D14">
+        <v>0.58604629999996405</v>
+      </c>
+      <c r="E14">
+        <v>0</v>
+      </c>
+      <c r="F14">
+        <v>9.1073796999999672</v>
+      </c>
+      <c r="G14">
+        <v>0.15795923000001721</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="C15">
+        <v>0.95895954000002348</v>
+      </c>
+      <c r="D15">
+        <v>4.3284704700000134</v>
+      </c>
+      <c r="E15">
+        <v>0</v>
+      </c>
+      <c r="F15">
+        <v>0.76945686999999907</v>
+      </c>
+      <c r="G15">
+        <v>0.28052963999999747</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="C16">
+        <v>0.9025624500000049</v>
+      </c>
+      <c r="D16">
+        <v>0.40407899000001635</v>
+      </c>
+      <c r="E16">
+        <v>0</v>
+      </c>
+      <c r="F16">
+        <v>0.91968800000000783</v>
+      </c>
+      <c r="G16">
+        <v>0.25344287000001486</v>
+      </c>
+    </row>
+    <row r="17" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C17">
+        <v>0.82973352999999861</v>
+      </c>
+      <c r="D17">
+        <v>0.10230470999999852</v>
+      </c>
+      <c r="E17">
+        <v>0</v>
+      </c>
+      <c r="F17">
+        <v>0.47302619999999251</v>
+      </c>
+      <c r="G17">
+        <v>3.5297200000172779E-3</v>
+      </c>
+    </row>
+    <row r="18" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C18">
+        <v>0.72779783999999381</v>
+      </c>
+      <c r="D18">
+        <v>0.15164471999997886</v>
+      </c>
+      <c r="E18">
+        <v>0</v>
+      </c>
+      <c r="F18">
+        <v>0.82643566999996665</v>
+      </c>
+      <c r="G18">
+        <v>0.1637938900000222</v>
+      </c>
+    </row>
+    <row r="19" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C19">
+        <v>0.8562303899999506</v>
+      </c>
+      <c r="D19">
+        <v>12.854483429999959</v>
+      </c>
+      <c r="E19">
+        <v>0</v>
+      </c>
+      <c r="F19">
+        <v>0.77448402999999644</v>
+      </c>
+      <c r="G19">
+        <v>0.21310288999995919</v>
+      </c>
+    </row>
+    <row r="20" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C20">
+        <v>0.42871243999996977</v>
+      </c>
+      <c r="D20">
+        <v>0.8775311899999565</v>
+      </c>
+      <c r="E20">
+        <v>0</v>
+      </c>
+      <c r="F20">
+        <v>0.3627410199999872</v>
+      </c>
+      <c r="G20">
+        <v>0.22846446999994896</v>
+      </c>
+    </row>
+    <row r="21" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C21">
+        <v>1.0084928599999898</v>
+      </c>
+      <c r="D21">
+        <v>0.2607821299999955</v>
+      </c>
+      <c r="E21">
+        <v>0</v>
+      </c>
+      <c r="F21">
+        <v>0.81527803000000176</v>
+      </c>
+      <c r="G21">
+        <v>0.13779650999998694</v>
+      </c>
+    </row>
+    <row r="22" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C22">
+        <v>1.6803902400000084</v>
+      </c>
+      <c r="D22">
+        <v>0.12377682999999706</v>
+      </c>
+      <c r="E22">
+        <v>0</v>
+      </c>
+      <c r="F22">
+        <v>1.1094856299999947</v>
+      </c>
+      <c r="G22">
+        <v>0.53419007999997348</v>
+      </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="C13:G13"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M16" sqref="M16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -1113,8 +1665,11 @@
       <c r="F1" s="1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G1" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -1133,8 +1688,11 @@
       <c r="F2" s="1">
         <v>1.8098528600000368</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G2" s="1">
+        <v>0.50085286000000728</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -1153,8 +1711,11 @@
       <c r="F3" s="1">
         <v>1.9193969400000146</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G3" s="1">
+        <v>0.66119541000000304</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -1173,8 +1734,11 @@
       <c r="F4" s="1">
         <v>1.9310206200000284</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G4" s="1">
+        <v>0.52589541000003059</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -1193,8 +1757,11 @@
       <c r="F5" s="1">
         <v>2.1676849899999997</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G5" s="1">
+        <v>0.77811976999998755</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -1213,8 +1780,11 @@
       <c r="F6" s="1">
         <v>2.0896359199999797</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G6" s="1">
+        <v>0.74120993999997431</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -1233,8 +1803,11 @@
       <c r="F7" s="1">
         <v>2.0464377299999814</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G7" s="1">
+        <v>0.18416543000000551</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>10</v>
       </c>
@@ -1253,8 +1826,11 @@
       <c r="F8" s="1">
         <v>1.9716071899999879</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G8" s="1">
+        <v>0.84466431000003972</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>11</v>
       </c>
@@ -1273,8 +1849,11 @@
       <c r="F9" s="1">
         <v>0.22118718000001714</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G9" s="1">
+        <v>0.50528071999997159</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>12</v>
       </c>
@@ -1293,8 +1872,11 @@
       <c r="F10" s="1">
         <v>2.1080673799999676</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G10" s="1">
+        <v>0.91106737999996135</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>13</v>
       </c>
@@ -1312,6 +1894,9 @@
       </c>
       <c r="F11" s="1">
         <v>2.0849101499999865</v>
+      </c>
+      <c r="G11" s="1">
+        <v>0.91791015000000975</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add scaling relation typesetting
</commit_message>
<xml_diff>
--- a/plotpackage/data/CO2RR.xlsx
+++ b/plotpackage/data/CO2RR.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7050" firstSheet="3" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7050" firstSheet="3" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="paral" sheetId="3" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="332" uniqueCount="37">
   <si>
     <t>*</t>
   </si>
@@ -1170,7 +1170,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
@@ -2282,15 +2282,15 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E37"/>
+  <dimension ref="A1:S37"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.35">
       <c r="B1" t="s">
         <v>24</v>
       </c>
@@ -2303,596 +2303,863 @@
       <c r="E1" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
+      <c r="P1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>1</v>
+      </c>
+      <c r="R1" t="s">
+        <v>2</v>
+      </c>
+      <c r="S1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B2">
-        <v>0</v>
-      </c>
-      <c r="C2">
+      <c r="B2" s="1">
+        <v>0</v>
+      </c>
+      <c r="C2" s="1">
         <v>0.84367677999994584</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="1">
         <v>0.21640443999995185</v>
       </c>
-      <c r="E2">
-        <v>0.12300000000000111</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
+      <c r="E2" s="1">
+        <v>0.12300000000000111</v>
+      </c>
+      <c r="O2" t="s">
+        <v>26</v>
+      </c>
+      <c r="P2">
+        <v>0</v>
+      </c>
+      <c r="Q2">
+        <v>0.84367677999994584</v>
+      </c>
+      <c r="R2">
+        <v>0.21640443999995185</v>
+      </c>
+      <c r="S2">
+        <v>0.12300000000000111</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A3" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="B3">
-        <v>0</v>
-      </c>
-      <c r="C3">
+      <c r="B3" s="1">
+        <v>0</v>
+      </c>
+      <c r="C3" s="1">
+        <v>0.3315079099999636</v>
+      </c>
+      <c r="D3" s="1">
+        <v>4.0126349999969335E-2</v>
+      </c>
+      <c r="E3" s="1">
+        <v>0.12300000000000111</v>
+      </c>
+      <c r="O3" t="s">
+        <v>27</v>
+      </c>
+      <c r="P3">
+        <v>0</v>
+      </c>
+      <c r="Q3">
         <v>2.618138999996944E-2</v>
       </c>
-      <c r="D3">
+      <c r="R3">
         <v>4.0126349999969335E-2</v>
       </c>
-      <c r="E3">
-        <v>0.12300000000000111</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
+      <c r="S3">
+        <v>0.12300000000000111</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A4" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B4">
-        <v>0</v>
-      </c>
-      <c r="C4">
+      <c r="B4" s="1">
+        <v>0</v>
+      </c>
+      <c r="C4" s="1">
+        <v>0.51077124999999768</v>
+      </c>
+      <c r="D4" s="1">
+        <v>-0.21640720000000258</v>
+      </c>
+      <c r="E4" s="1">
+        <v>0.12300000000000111</v>
+      </c>
+      <c r="O4" t="s">
+        <v>12</v>
+      </c>
+      <c r="P4">
+        <v>0</v>
+      </c>
+      <c r="Q4">
         <v>0.52069346999996213</v>
       </c>
-      <c r="D4">
+      <c r="R4">
         <v>-0.21640720000000258</v>
       </c>
-      <c r="E4">
-        <v>0.12300000000000111</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
+      <c r="S4">
+        <v>0.12300000000000111</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B5">
-        <v>0</v>
-      </c>
-      <c r="C5">
+      <c r="B5" s="1">
+        <v>0</v>
+      </c>
+      <c r="C5" s="1">
         <v>0.49457561000001959</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="1">
         <v>-0.50070746000001165</v>
       </c>
-      <c r="E5">
-        <v>0.12300000000000111</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
+      <c r="E5" s="1">
+        <v>0.12300000000000111</v>
+      </c>
+      <c r="O5" t="s">
+        <v>7</v>
+      </c>
+      <c r="P5">
+        <v>0</v>
+      </c>
+      <c r="Q5">
+        <v>0.49457561000001959</v>
+      </c>
+      <c r="R5">
+        <v>-0.50070746000001165</v>
+      </c>
+      <c r="S5">
+        <v>0.12300000000000111</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A6" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B6">
-        <v>0</v>
-      </c>
-      <c r="C6">
+      <c r="B6" s="1">
+        <v>0</v>
+      </c>
+      <c r="C6" s="1">
         <v>0.12548745000002981</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="1">
         <v>-0.7313844799999849</v>
       </c>
-      <c r="E6">
-        <v>0.12300000000000111</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
+      <c r="E6" s="1">
+        <v>0.12300000000000111</v>
+      </c>
+      <c r="O6" t="s">
+        <v>9</v>
+      </c>
+      <c r="P6">
+        <v>0</v>
+      </c>
+      <c r="Q6">
+        <v>0.12548745000002981</v>
+      </c>
+      <c r="R6">
+        <v>-0.7313844799999849</v>
+      </c>
+      <c r="S6">
+        <v>0.12300000000000111</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A7" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B7">
-        <v>0</v>
-      </c>
-      <c r="C7">
+      <c r="B7" s="1">
+        <v>0</v>
+      </c>
+      <c r="C7" s="1">
         <v>0.25444276999996163</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="1">
         <v>-0.77851690000001028</v>
       </c>
-      <c r="E7">
-        <v>0.12300000000000111</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
+      <c r="E7" s="1">
+        <v>0.12300000000000111</v>
+      </c>
+      <c r="O7" t="s">
+        <v>10</v>
+      </c>
+      <c r="P7">
+        <v>0</v>
+      </c>
+      <c r="Q7">
+        <v>0.25444276999996163</v>
+      </c>
+      <c r="R7">
+        <v>-0.77851690000001028</v>
+      </c>
+      <c r="S7">
+        <v>0.12300000000000111</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B8">
-        <v>0</v>
-      </c>
-      <c r="C8">
+      <c r="B8" s="1">
+        <v>0</v>
+      </c>
+      <c r="C8" s="1">
         <v>0.88424493000001547</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="1">
         <v>-0.32130351000001767</v>
       </c>
-      <c r="E8">
-        <v>0.12300000000000111</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
+      <c r="E8" s="1">
+        <v>0.12300000000000111</v>
+      </c>
+      <c r="O8" t="s">
+        <v>6</v>
+      </c>
+      <c r="P8">
+        <v>0</v>
+      </c>
+      <c r="Q8">
+        <v>0.88424493000001547</v>
+      </c>
+      <c r="R8">
+        <v>-0.32130351000001767</v>
+      </c>
+      <c r="S8">
+        <v>0.12300000000000111</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A9" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B9">
-        <v>0</v>
-      </c>
-      <c r="C9">
+      <c r="B9" s="1">
+        <v>0</v>
+      </c>
+      <c r="C9" s="1">
         <v>1.0889947399999684</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="1">
         <v>8.500547999999597E-2</v>
       </c>
-      <c r="E9">
-        <v>0.12300000000000111</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
+      <c r="E9" s="1">
+        <v>0.12300000000000111</v>
+      </c>
+      <c r="O9" t="s">
+        <v>5</v>
+      </c>
+      <c r="P9">
+        <v>0</v>
+      </c>
+      <c r="Q9">
+        <v>1.0889947399999684</v>
+      </c>
+      <c r="R9">
+        <v>8.500547999999597E-2</v>
+      </c>
+      <c r="S9">
+        <v>0.12300000000000111</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A10" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="B10">
-        <v>0</v>
-      </c>
-      <c r="C10">
+      <c r="B10" s="1">
+        <v>0</v>
+      </c>
+      <c r="C10" s="1">
         <v>1.6351955700000005</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="1">
         <v>0.3263979700000057</v>
       </c>
-      <c r="E10">
-        <v>0.12300000000000111</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
+      <c r="E10" s="1">
+        <v>0.12300000000000111</v>
+      </c>
+      <c r="O10" t="s">
+        <v>28</v>
+      </c>
+      <c r="P10">
+        <v>0</v>
+      </c>
+      <c r="Q10">
+        <v>1.6351955700000005</v>
+      </c>
+      <c r="R10">
+        <v>0.3263979700000057</v>
+      </c>
+      <c r="S10">
+        <v>0.12300000000000111</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A11" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="B11">
-        <v>0</v>
-      </c>
-      <c r="C11">
+      <c r="B11" s="1">
+        <v>0</v>
+      </c>
+      <c r="C11" s="1">
         <v>0.95501516000000919</v>
       </c>
-      <c r="D11">
+      <c r="D11" s="1">
         <v>0.46510843999998386</v>
       </c>
-      <c r="E11">
-        <v>0.12300000000000111</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
+      <c r="E11" s="1">
+        <v>0.12300000000000111</v>
+      </c>
+      <c r="O11" t="s">
+        <v>29</v>
+      </c>
+      <c r="P11">
+        <v>0</v>
+      </c>
+      <c r="Q11">
+        <v>0.95501516000000919</v>
+      </c>
+      <c r="R11">
+        <v>0.46510843999998386</v>
+      </c>
+      <c r="S11">
+        <v>0.12300000000000111</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A12" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="B12">
-        <v>0</v>
-      </c>
-      <c r="C12">
+      <c r="B12" s="1">
+        <v>0</v>
+      </c>
+      <c r="C12" s="1">
         <v>-2.3544356900000096</v>
       </c>
-      <c r="D12">
+      <c r="D12" s="1">
         <v>-2.2372229899999745</v>
       </c>
-      <c r="E12">
-        <v>0.12300000000000111</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
+      <c r="E12" s="1">
+        <v>0.12300000000000111</v>
+      </c>
+      <c r="O12" t="s">
+        <v>30</v>
+      </c>
+      <c r="P12">
+        <v>0</v>
+      </c>
+      <c r="Q12">
+        <v>-2.3544356900000096</v>
+      </c>
+      <c r="R12">
+        <v>-2.2372229899999745</v>
+      </c>
+      <c r="S12">
+        <v>0.12300000000000111</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A13" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="B13">
-        <v>0</v>
-      </c>
-      <c r="C13">
+      <c r="B13" s="1">
+        <v>0</v>
+      </c>
+      <c r="C13" s="1">
         <v>-1.0355091500000029</v>
       </c>
-      <c r="D13">
+      <c r="D13" s="1">
+        <v>0.47704434999996082</v>
+      </c>
+      <c r="E13" s="1">
+        <v>0.12300000000000111</v>
+      </c>
+      <c r="O13" t="s">
+        <v>31</v>
+      </c>
+      <c r="P13">
+        <v>0</v>
+      </c>
+      <c r="Q13">
+        <v>-1.0355091500000029</v>
+      </c>
+      <c r="R13">
         <v>-0.69508848000004875</v>
       </c>
-      <c r="E13">
-        <v>0.12300000000000111</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
+      <c r="S13">
+        <v>0.12300000000000111</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A14" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B14">
-        <v>0</v>
-      </c>
-      <c r="C14">
+      <c r="B14" s="1">
+        <v>0</v>
+      </c>
+      <c r="C14" s="1">
         <v>0.56285378000000463</v>
       </c>
-      <c r="D14">
+      <c r="D14" s="1">
         <v>-0.36565296999999575</v>
       </c>
-      <c r="E14">
-        <v>0.12300000000000111</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A15" t="s">
+      <c r="E14" s="1">
+        <v>0.12300000000000111</v>
+      </c>
+      <c r="O14" t="s">
+        <v>32</v>
+      </c>
+      <c r="P14">
+        <v>0</v>
+      </c>
+      <c r="Q14">
+        <v>0.56285378000000463</v>
+      </c>
+      <c r="R14">
+        <v>-0.36565296999999575</v>
+      </c>
+      <c r="S14">
+        <v>0.12300000000000111</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A15" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B15">
-        <v>0</v>
-      </c>
-      <c r="C15">
+      <c r="B15" s="1">
+        <v>0</v>
+      </c>
+      <c r="C15" s="1">
         <v>0.53497151999999204</v>
       </c>
-      <c r="D15">
+      <c r="D15" s="1">
         <v>-0.18208612999996987</v>
       </c>
-      <c r="E15">
-        <v>0.12300000000000111</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A16" t="s">
+      <c r="E15" s="1">
+        <v>0.12300000000000111</v>
+      </c>
+      <c r="O15" t="s">
+        <v>33</v>
+      </c>
+      <c r="P15">
+        <v>0</v>
+      </c>
+      <c r="Q15">
+        <v>0.53497151999999204</v>
+      </c>
+      <c r="R15">
+        <v>-0.18208612999996987</v>
+      </c>
+      <c r="S15">
+        <v>0.12300000000000111</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A16" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B16">
-        <v>0</v>
-      </c>
-      <c r="C16">
+      <c r="B16" s="1">
+        <v>0</v>
+      </c>
+      <c r="C16" s="1">
         <v>0.74170350999997225</v>
       </c>
-      <c r="D16">
+      <c r="D16" s="1">
         <v>-0.62919791000002689</v>
       </c>
-      <c r="E16">
-        <v>0.12300000000000111</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A17" t="s">
+      <c r="E16" s="1">
+        <v>0.12300000000000111</v>
+      </c>
+      <c r="O16" t="s">
+        <v>34</v>
+      </c>
+      <c r="P16">
+        <v>0</v>
+      </c>
+      <c r="Q16">
+        <v>0.74170350999997225</v>
+      </c>
+      <c r="R16">
+        <v>-0.62919791000002689</v>
+      </c>
+      <c r="S16">
+        <v>0.12300000000000111</v>
+      </c>
+    </row>
+    <row r="17" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A17" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B17">
-        <v>0</v>
-      </c>
-      <c r="C17">
+      <c r="B17" s="1">
+        <v>0</v>
+      </c>
+      <c r="C17" s="1">
         <v>0.94914526999996696</v>
       </c>
-      <c r="D17">
+      <c r="D17" s="1">
         <v>-9.5206500000028171E-2</v>
       </c>
-      <c r="E17">
-        <v>0.12300000000000111</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A18" t="s">
+      <c r="E17" s="1">
+        <v>0.12300000000000111</v>
+      </c>
+      <c r="O17" t="s">
+        <v>35</v>
+      </c>
+      <c r="P17">
+        <v>0</v>
+      </c>
+      <c r="Q17">
+        <v>0.94914526999996696</v>
+      </c>
+      <c r="R17">
+        <v>-9.5206500000028171E-2</v>
+      </c>
+      <c r="S17">
+        <v>0.12300000000000111</v>
+      </c>
+    </row>
+    <row r="18" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A18" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="B18">
-        <v>0</v>
-      </c>
-      <c r="C18">
+      <c r="B18" s="1">
+        <v>0</v>
+      </c>
+      <c r="C18" s="1">
+        <v>1.9851872199999931</v>
+      </c>
+      <c r="D18" s="1">
+        <v>0.48779698999998189</v>
+      </c>
+      <c r="E18" s="1">
+        <v>0.12300000000000111</v>
+      </c>
+      <c r="O18" t="s">
+        <v>36</v>
+      </c>
+      <c r="P18">
+        <v>0</v>
+      </c>
+      <c r="Q18">
         <v>1.9843051699999634</v>
       </c>
-      <c r="D18">
+      <c r="R18">
         <v>0.48650724999997763</v>
       </c>
-      <c r="E18">
-        <v>0.12300000000000111</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B20" t="s">
+      <c r="S18">
+        <v>0.12300000000000111</v>
+      </c>
+    </row>
+    <row r="20" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="P20" t="s">
         <v>24</v>
       </c>
-      <c r="C20" t="s">
+      <c r="Q20" t="s">
         <v>1</v>
       </c>
-      <c r="D20" t="s">
+      <c r="R20" t="s">
         <v>2</v>
       </c>
-      <c r="E20" t="s">
+      <c r="S20" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A21" s="1" t="s">
+    <row r="21" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="O21" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B21" s="1">
-        <v>0</v>
-      </c>
-      <c r="C21" s="1">
+      <c r="P21" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q21" s="1">
         <v>0.84367677999994584</v>
       </c>
-      <c r="D21" s="1">
+      <c r="R21" s="1">
         <v>0.21640443999995185</v>
       </c>
-      <c r="E21" s="1">
-        <v>0.12300000000000111</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A22" s="5" t="s">
+      <c r="S21" s="1">
+        <v>0.12300000000000111</v>
+      </c>
+    </row>
+    <row r="22" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="O22" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="B22" s="1">
-        <v>0</v>
-      </c>
-      <c r="C22" s="1">
+      <c r="P22" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q22" s="1">
         <v>0.3315079099999636</v>
       </c>
-      <c r="D22" s="1">
+      <c r="R22" s="1">
         <v>4.0126349999969335E-2</v>
       </c>
-      <c r="E22" s="1">
-        <v>0.12300000000000111</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A23" s="5" t="s">
+      <c r="S22" s="1">
+        <v>0.12300000000000111</v>
+      </c>
+    </row>
+    <row r="23" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="O23" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B23" s="1">
-        <v>0</v>
-      </c>
-      <c r="C23" s="1">
+      <c r="P23" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q23" s="1">
         <v>0.51077124999999768</v>
       </c>
-      <c r="D23" s="1">
+      <c r="R23" s="1">
         <v>-0.21640720000000258</v>
       </c>
-      <c r="E23" s="1">
-        <v>0.12300000000000111</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A24" s="1" t="s">
+      <c r="S23" s="1">
+        <v>0.12300000000000111</v>
+      </c>
+    </row>
+    <row r="24" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="O24" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B24" s="1">
-        <v>0</v>
-      </c>
-      <c r="C24" s="1">
+      <c r="P24" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q24" s="1">
         <v>0.49457561000001959</v>
       </c>
-      <c r="D24" s="1">
+      <c r="R24" s="1">
         <v>-0.50070746000001165</v>
       </c>
-      <c r="E24" s="1">
-        <v>0.12300000000000111</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A25" s="1" t="s">
+      <c r="S24" s="1">
+        <v>0.12300000000000111</v>
+      </c>
+    </row>
+    <row r="25" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="O25" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B25" s="1">
-        <v>0</v>
-      </c>
-      <c r="C25" s="1">
+      <c r="P25" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q25" s="1">
         <v>0.12548745000002981</v>
       </c>
-      <c r="D25" s="1">
+      <c r="R25" s="1">
         <v>-0.7313844799999849</v>
       </c>
-      <c r="E25" s="1">
-        <v>0.12300000000000111</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A26" s="1" t="s">
+      <c r="S25" s="1">
+        <v>0.12300000000000111</v>
+      </c>
+    </row>
+    <row r="26" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="O26" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B26" s="1">
-        <v>0</v>
-      </c>
-      <c r="C26" s="1">
+      <c r="P26" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q26" s="1">
         <v>0.25444276999996163</v>
       </c>
-      <c r="D26" s="1">
+      <c r="R26" s="1">
         <v>-0.77851690000001028</v>
       </c>
-      <c r="E26" s="1">
-        <v>0.12300000000000111</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A27" s="1" t="s">
+      <c r="S26" s="1">
+        <v>0.12300000000000111</v>
+      </c>
+    </row>
+    <row r="27" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="O27" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B27" s="1">
-        <v>0</v>
-      </c>
-      <c r="C27" s="1">
+      <c r="P27" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q27" s="1">
         <v>0.88424493000001547</v>
       </c>
-      <c r="D27" s="1">
+      <c r="R27" s="1">
         <v>-0.32130351000001767</v>
       </c>
-      <c r="E27" s="1">
-        <v>0.12300000000000111</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A28" s="1" t="s">
+      <c r="S27" s="1">
+        <v>0.12300000000000111</v>
+      </c>
+    </row>
+    <row r="28" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="O28" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B28" s="1">
-        <v>0</v>
-      </c>
-      <c r="C28" s="1">
+      <c r="P28" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q28" s="1">
         <v>1.0889947399999684</v>
       </c>
-      <c r="D28" s="1">
+      <c r="R28" s="1">
         <v>8.500547999999597E-2</v>
       </c>
-      <c r="E28" s="1">
-        <v>0.12300000000000111</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A29" s="5" t="s">
+      <c r="S28" s="1">
+        <v>0.12300000000000111</v>
+      </c>
+    </row>
+    <row r="29" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="O29" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="B29" s="1">
-        <v>0</v>
-      </c>
-      <c r="C29" s="1">
+      <c r="P29" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q29" s="1">
         <v>1.6351955700000005</v>
       </c>
-      <c r="D29" s="1">
+      <c r="R29" s="1">
         <v>0.3263979700000057</v>
       </c>
-      <c r="E29" s="1">
-        <v>0.12300000000000111</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A30" s="5" t="s">
+      <c r="S29" s="1">
+        <v>0.12300000000000111</v>
+      </c>
+    </row>
+    <row r="30" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="O30" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="B30" s="1">
-        <v>0</v>
-      </c>
-      <c r="C30" s="1">
+      <c r="P30" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q30" s="1">
         <v>0.95501516000000919</v>
       </c>
-      <c r="D30" s="1">
+      <c r="R30" s="1">
         <v>0.46510843999998386</v>
       </c>
-      <c r="E30" s="1">
-        <v>0.12300000000000111</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A31" s="5" t="s">
+      <c r="S30" s="1">
+        <v>0.12300000000000111</v>
+      </c>
+    </row>
+    <row r="31" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="O31" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="B31" s="1">
-        <v>0</v>
-      </c>
-      <c r="C31" s="1">
+      <c r="P31" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q31" s="1">
         <v>-2.3544356900000096</v>
       </c>
-      <c r="D31" s="1">
+      <c r="R31" s="1">
         <v>-2.2372229899999745</v>
       </c>
-      <c r="E31" s="1">
-        <v>0.12300000000000111</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A32" s="5" t="s">
+      <c r="S31" s="1">
+        <v>0.12300000000000111</v>
+      </c>
+    </row>
+    <row r="32" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="O32" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="B32" s="1">
-        <v>0</v>
-      </c>
-      <c r="C32" s="1">
+      <c r="P32" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q32" s="1">
         <v>-1.0355091500000029</v>
       </c>
-      <c r="D32" s="1">
+      <c r="R32" s="1">
         <v>0.47704434999996082</v>
       </c>
-      <c r="E32" s="1">
-        <v>0.12300000000000111</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A33" s="1" t="s">
+      <c r="S32" s="1">
+        <v>0.12300000000000111</v>
+      </c>
+    </row>
+    <row r="33" spans="15:19" x14ac:dyDescent="0.35">
+      <c r="O33" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B33" s="1">
-        <v>0</v>
-      </c>
-      <c r="C33" s="1">
+      <c r="P33" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q33" s="1">
         <v>0.56285378000000463</v>
       </c>
-      <c r="D33" s="1">
+      <c r="R33" s="1">
         <v>-0.36565296999999575</v>
       </c>
-      <c r="E33" s="1">
-        <v>0.12300000000000111</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A34" s="1" t="s">
+      <c r="S33" s="1">
+        <v>0.12300000000000111</v>
+      </c>
+    </row>
+    <row r="34" spans="15:19" x14ac:dyDescent="0.35">
+      <c r="O34" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B34" s="1">
-        <v>0</v>
-      </c>
-      <c r="C34" s="1">
+      <c r="P34" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q34" s="1">
         <v>0.53497151999999204</v>
       </c>
-      <c r="D34" s="1">
+      <c r="R34" s="1">
         <v>-0.18208612999996987</v>
       </c>
-      <c r="E34" s="1">
-        <v>0.12300000000000111</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A35" s="1" t="s">
+      <c r="S34" s="1">
+        <v>0.12300000000000111</v>
+      </c>
+    </row>
+    <row r="35" spans="15:19" x14ac:dyDescent="0.35">
+      <c r="O35" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B35" s="1">
-        <v>0</v>
-      </c>
-      <c r="C35" s="1">
+      <c r="P35" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q35" s="1">
         <v>0.74170350999997225</v>
       </c>
-      <c r="D35" s="1">
+      <c r="R35" s="1">
         <v>-0.62919791000002689</v>
       </c>
-      <c r="E35" s="1">
-        <v>0.12300000000000111</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A36" s="1" t="s">
+      <c r="S35" s="1">
+        <v>0.12300000000000111</v>
+      </c>
+    </row>
+    <row r="36" spans="15:19" x14ac:dyDescent="0.35">
+      <c r="O36" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B36" s="1">
-        <v>0</v>
-      </c>
-      <c r="C36" s="1">
+      <c r="P36" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q36" s="1">
         <v>0.94914526999996696</v>
       </c>
-      <c r="D36" s="1">
+      <c r="R36" s="1">
         <v>-9.5206500000028171E-2</v>
       </c>
-      <c r="E36" s="1">
-        <v>0.12300000000000111</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A37" s="5" t="s">
+      <c r="S36" s="1">
+        <v>0.12300000000000111</v>
+      </c>
+    </row>
+    <row r="37" spans="15:19" x14ac:dyDescent="0.35">
+      <c r="O37" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="B37" s="1">
-        <v>0</v>
-      </c>
-      <c r="C37" s="1">
+      <c r="P37" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q37" s="1">
         <v>1.9851872199999931</v>
       </c>
-      <c r="D37" s="1">
+      <c r="R37" s="1">
         <v>0.48779698999998189</v>
       </c>
-      <c r="E37" s="1">
+      <c r="S37" s="1">
         <v>0.12300000000000111</v>
       </c>
     </row>
@@ -2903,15 +3170,15 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E37"/>
+  <dimension ref="A1:S37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="H27" sqref="H27"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.35">
       <c r="B1" t="s">
         <v>24</v>
       </c>
@@ -2924,596 +3191,863 @@
       <c r="E1" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
+      <c r="P1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>1</v>
+      </c>
+      <c r="R1" t="s">
+        <v>2</v>
+      </c>
+      <c r="S1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B2">
-        <v>0</v>
-      </c>
-      <c r="C2">
+      <c r="B2" s="1">
+        <v>0</v>
+      </c>
+      <c r="C2" s="1">
         <v>0.84367677999994584</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="1">
         <v>0.21640443999995185</v>
       </c>
-      <c r="E2">
-        <v>0.12300000000000111</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
+      <c r="E2" s="1">
+        <v>0.12300000000000111</v>
+      </c>
+      <c r="O2" t="s">
+        <v>26</v>
+      </c>
+      <c r="P2">
+        <v>0</v>
+      </c>
+      <c r="Q2">
+        <v>0.84367677999994584</v>
+      </c>
+      <c r="R2">
+        <v>0.21640443999995185</v>
+      </c>
+      <c r="S2">
+        <v>0.12300000000000111</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A3" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="B3">
-        <v>0</v>
-      </c>
-      <c r="C3">
+      <c r="B3" s="1">
+        <v>0</v>
+      </c>
+      <c r="C3" s="1">
         <v>0.20492825999996711</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="1">
+        <v>3.1399299999964825E-2</v>
+      </c>
+      <c r="E3" s="1">
+        <v>0.12300000000000111</v>
+      </c>
+      <c r="O3" t="s">
+        <v>27</v>
+      </c>
+      <c r="P3">
+        <v>0</v>
+      </c>
+      <c r="Q3">
+        <v>0.20492825999996711</v>
+      </c>
+      <c r="R3">
         <v>-0.29827053999998654</v>
       </c>
-      <c r="E3">
-        <v>0.12300000000000111</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
+      <c r="S3">
+        <v>0.12300000000000111</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A4" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B4">
-        <v>0</v>
-      </c>
-      <c r="C4">
+      <c r="B4" s="1">
+        <v>0</v>
+      </c>
+      <c r="C4" s="1">
         <v>0.50867605999996357</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="1">
         <v>-0.14474954000003137</v>
       </c>
-      <c r="E4">
-        <v>0.12300000000000111</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
+      <c r="E4" s="1">
+        <v>0.12300000000000111</v>
+      </c>
+      <c r="O4" t="s">
+        <v>12</v>
+      </c>
+      <c r="P4">
+        <v>0</v>
+      </c>
+      <c r="Q4">
+        <v>0.50867605999996357</v>
+      </c>
+      <c r="R4">
+        <v>-0.14474954000003137</v>
+      </c>
+      <c r="S4">
+        <v>0.12300000000000111</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A5" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B5">
-        <v>0</v>
-      </c>
-      <c r="C5">
+      <c r="B5" s="1">
+        <v>0</v>
+      </c>
+      <c r="C5" s="1">
         <v>0.59255065000001395</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="1">
         <v>-0.33148215000001002</v>
       </c>
-      <c r="E5">
-        <v>0.12300000000000111</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
+      <c r="E5" s="1">
+        <v>0.12300000000000111</v>
+      </c>
+      <c r="O5" t="s">
+        <v>7</v>
+      </c>
+      <c r="P5">
+        <v>0</v>
+      </c>
+      <c r="Q5">
+        <v>0.59255065000001395</v>
+      </c>
+      <c r="R5">
+        <v>-0.33148215000001002</v>
+      </c>
+      <c r="S5">
+        <v>0.12300000000000111</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A6" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B6">
-        <v>0</v>
-      </c>
-      <c r="C6">
+      <c r="B6" s="1">
+        <v>0</v>
+      </c>
+      <c r="C6" s="1">
         <v>0.50554635000002435</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="1">
         <v>-0.6216317699999756</v>
       </c>
-      <c r="E6">
-        <v>0.12300000000000111</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
+      <c r="E6" s="1">
+        <v>0.12300000000000111</v>
+      </c>
+      <c r="O6" t="s">
+        <v>9</v>
+      </c>
+      <c r="P6">
+        <v>0</v>
+      </c>
+      <c r="Q6">
+        <v>0.50554635000002435</v>
+      </c>
+      <c r="R6">
+        <v>-0.6216317699999756</v>
+      </c>
+      <c r="S6">
+        <v>0.12300000000000111</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A7" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B7">
-        <v>0</v>
-      </c>
-      <c r="C7">
+      <c r="B7" s="1">
+        <v>0</v>
+      </c>
+      <c r="C7" s="1">
         <v>0.89115173999999087</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="1">
         <v>-0.65971805999999944</v>
       </c>
-      <c r="E7">
-        <v>0.12300000000000111</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
+      <c r="E7" s="1">
+        <v>0.12300000000000111</v>
+      </c>
+      <c r="O7" t="s">
+        <v>10</v>
+      </c>
+      <c r="P7">
+        <v>0</v>
+      </c>
+      <c r="Q7">
+        <v>0.89115173999999087</v>
+      </c>
+      <c r="R7">
+        <v>-0.65971805999999944</v>
+      </c>
+      <c r="S7">
+        <v>0.12300000000000111</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B8">
-        <v>0</v>
-      </c>
-      <c r="C8">
+      <c r="B8" s="1">
+        <v>0</v>
+      </c>
+      <c r="C8" s="1">
         <v>0.62801460999997261</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="1">
         <v>-0.52560204000003452</v>
       </c>
-      <c r="E8">
-        <v>0.12300000000000111</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
+      <c r="E8" s="1">
+        <v>0.12300000000000111</v>
+      </c>
+      <c r="O8" t="s">
+        <v>6</v>
+      </c>
+      <c r="P8">
+        <v>0</v>
+      </c>
+      <c r="Q8">
+        <v>0.62801460999997261</v>
+      </c>
+      <c r="R8">
+        <v>-0.52560204000003452</v>
+      </c>
+      <c r="S8">
+        <v>0.12300000000000111</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A9" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B9">
-        <v>0</v>
-      </c>
-      <c r="C9">
+      <c r="B9" s="1">
+        <v>0</v>
+      </c>
+      <c r="C9" s="1">
         <v>1.0472342099999921</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="1">
         <v>3.4994419999964776E-2</v>
       </c>
-      <c r="E9">
-        <v>0.12300000000000111</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
+      <c r="E9" s="1">
+        <v>0.12300000000000111</v>
+      </c>
+      <c r="O9" t="s">
+        <v>5</v>
+      </c>
+      <c r="P9">
+        <v>0</v>
+      </c>
+      <c r="Q9">
+        <v>1.0472342099999921</v>
+      </c>
+      <c r="R9">
+        <v>3.4994419999964776E-2</v>
+      </c>
+      <c r="S9">
+        <v>0.12300000000000111</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A10" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B10">
-        <v>0</v>
-      </c>
-      <c r="C10">
+      <c r="B10" s="1">
+        <v>0</v>
+      </c>
+      <c r="C10" s="1">
         <v>1.6170278100000175</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="1">
         <v>0.37293717999999743</v>
       </c>
-      <c r="E10">
-        <v>0.12300000000000111</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
+      <c r="E10" s="1">
+        <v>0.12300000000000111</v>
+      </c>
+      <c r="O10" t="s">
+        <v>28</v>
+      </c>
+      <c r="P10">
+        <v>0</v>
+      </c>
+      <c r="Q10">
+        <v>1.6170278100000175</v>
+      </c>
+      <c r="R10">
+        <v>0.37293717999999743</v>
+      </c>
+      <c r="S10">
+        <v>0.12300000000000111</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A11" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="B11">
-        <v>0</v>
-      </c>
-      <c r="C11">
+      <c r="B11" s="1">
+        <v>0</v>
+      </c>
+      <c r="C11" s="1">
+        <v>0.86854102000000211</v>
+      </c>
+      <c r="D11" s="1">
+        <v>0.45489865999995871</v>
+      </c>
+      <c r="E11" s="1">
+        <v>0.12300000000000111</v>
+      </c>
+      <c r="O11" t="s">
+        <v>29</v>
+      </c>
+      <c r="P11">
+        <v>0</v>
+      </c>
+      <c r="Q11">
         <v>0.85332067000000933</v>
       </c>
-      <c r="D11">
+      <c r="R11">
         <v>0.41119889999997739</v>
       </c>
-      <c r="E11">
-        <v>0.12300000000000111</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
+      <c r="S11">
+        <v>0.12300000000000111</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A12" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="B12">
-        <v>0</v>
-      </c>
-      <c r="C12">
+      <c r="B12" s="1">
+        <v>0</v>
+      </c>
+      <c r="C12" s="1">
+        <v>-0.18472628000001379</v>
+      </c>
+      <c r="D12" s="1">
+        <v>4.0702499999731856E-3</v>
+      </c>
+      <c r="E12" s="1">
+        <v>0.12300000000000111</v>
+      </c>
+      <c r="O12" t="s">
+        <v>30</v>
+      </c>
+      <c r="P12">
+        <v>0</v>
+      </c>
+      <c r="Q12">
         <v>-6.8367130000019927E-2</v>
       </c>
-      <c r="D12">
+      <c r="R12">
         <v>0.11426077999998441</v>
       </c>
-      <c r="E12">
-        <v>0.12300000000000111</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
+      <c r="S12">
+        <v>0.12300000000000111</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A13" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="B13">
-        <v>0</v>
-      </c>
-      <c r="C13">
+      <c r="B13" s="1">
+        <v>0</v>
+      </c>
+      <c r="C13" s="1">
+        <v>0.4962419299999894</v>
+      </c>
+      <c r="D13" s="1">
+        <v>-0.12233271999998507</v>
+      </c>
+      <c r="E13" s="1">
+        <v>0.12300000000000111</v>
+      </c>
+      <c r="O13" t="s">
+        <v>31</v>
+      </c>
+      <c r="P13">
+        <v>0</v>
+      </c>
+      <c r="Q13">
         <v>0.61638396000000029</v>
       </c>
-      <c r="D13">
+      <c r="R13">
         <v>-0.11936635000001772</v>
       </c>
-      <c r="E13">
-        <v>0.12300000000000111</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
+      <c r="S13">
+        <v>0.12300000000000111</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A14" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="B14">
-        <v>0</v>
-      </c>
-      <c r="C14">
+      <c r="B14" s="1">
+        <v>0</v>
+      </c>
+      <c r="C14" s="1">
+        <v>0.54488558999997139</v>
+      </c>
+      <c r="D14" s="1">
+        <v>-0.19933409999999796</v>
+      </c>
+      <c r="E14" s="1">
+        <v>0.12300000000000111</v>
+      </c>
+      <c r="O14" t="s">
+        <v>32</v>
+      </c>
+      <c r="P14">
+        <v>0</v>
+      </c>
+      <c r="Q14">
         <v>0.54131256999999522</v>
       </c>
-      <c r="D14">
+      <c r="R14">
         <v>-0.19933409999999796</v>
       </c>
-      <c r="E14">
-        <v>0.12300000000000111</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A15" t="s">
+      <c r="S14">
+        <v>0.12300000000000111</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A15" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B15">
-        <v>0</v>
-      </c>
-      <c r="C15">
+      <c r="B15" s="1">
+        <v>0</v>
+      </c>
+      <c r="C15" s="1">
         <v>0.33292057999999969</v>
       </c>
-      <c r="D15">
+      <c r="D15" s="1">
         <v>-0.48480682000002773</v>
       </c>
-      <c r="E15">
-        <v>0.12300000000000111</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A16" t="s">
+      <c r="E15" s="1">
+        <v>0.12300000000000111</v>
+      </c>
+      <c r="O15" t="s">
+        <v>33</v>
+      </c>
+      <c r="P15">
+        <v>0</v>
+      </c>
+      <c r="Q15">
+        <v>0.33292057999999969</v>
+      </c>
+      <c r="R15">
+        <v>-0.48480682000002773</v>
+      </c>
+      <c r="S15">
+        <v>0.12300000000000111</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A16" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B16">
-        <v>0</v>
-      </c>
-      <c r="C16">
+      <c r="B16" s="1">
+        <v>0</v>
+      </c>
+      <c r="C16" s="1">
         <v>0.71068052999998343</v>
       </c>
-      <c r="D16">
+      <c r="D16" s="1">
         <v>-0.7608479800000616</v>
       </c>
-      <c r="E16">
-        <v>0.12300000000000111</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A17" t="s">
+      <c r="E16" s="1">
+        <v>0.12300000000000111</v>
+      </c>
+      <c r="O16" t="s">
+        <v>34</v>
+      </c>
+      <c r="P16">
+        <v>0</v>
+      </c>
+      <c r="Q16">
+        <v>0.71068052999998343</v>
+      </c>
+      <c r="R16">
+        <v>-0.7608479800000616</v>
+      </c>
+      <c r="S16">
+        <v>0.12300000000000111</v>
+      </c>
+    </row>
+    <row r="17" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A17" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B17">
-        <v>0</v>
-      </c>
-      <c r="C17">
+      <c r="B17" s="1">
+        <v>0</v>
+      </c>
+      <c r="C17" s="1">
         <v>0.90776295999994971</v>
       </c>
-      <c r="D17">
+      <c r="D17" s="1">
         <v>-0.15853684000002133</v>
       </c>
-      <c r="E17">
-        <v>0.12300000000000111</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A18" t="s">
+      <c r="E17" s="1">
+        <v>0.12300000000000111</v>
+      </c>
+      <c r="O17" t="s">
+        <v>35</v>
+      </c>
+      <c r="P17">
+        <v>0</v>
+      </c>
+      <c r="Q17">
+        <v>0.90776295999994971</v>
+      </c>
+      <c r="R17">
+        <v>-0.15853684000002133</v>
+      </c>
+      <c r="S17">
+        <v>0.12300000000000111</v>
+      </c>
+    </row>
+    <row r="18" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A18" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B18">
-        <v>0</v>
-      </c>
-      <c r="C18">
+      <c r="B18" s="1">
+        <v>0</v>
+      </c>
+      <c r="C18" s="1">
         <v>1.9748885499999957</v>
       </c>
-      <c r="D18">
+      <c r="D18" s="1">
         <v>0.47546450000003304</v>
       </c>
-      <c r="E18">
-        <v>0.12300000000000111</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B20" t="s">
+      <c r="E18" s="1">
+        <v>0.12300000000000111</v>
+      </c>
+      <c r="O18" t="s">
+        <v>36</v>
+      </c>
+      <c r="P18">
+        <v>0</v>
+      </c>
+      <c r="Q18">
+        <v>1.9748885499999957</v>
+      </c>
+      <c r="R18">
+        <v>0.47546450000003304</v>
+      </c>
+      <c r="S18">
+        <v>0.12300000000000111</v>
+      </c>
+    </row>
+    <row r="20" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="P20" t="s">
         <v>24</v>
       </c>
-      <c r="C20" t="s">
+      <c r="Q20" t="s">
         <v>1</v>
       </c>
-      <c r="D20" t="s">
+      <c r="R20" t="s">
         <v>2</v>
       </c>
-      <c r="E20" t="s">
+      <c r="S20" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A21" s="1" t="s">
+    <row r="21" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="O21" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B21" s="1">
-        <v>0</v>
-      </c>
-      <c r="C21" s="1">
+      <c r="P21" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q21" s="1">
         <v>0.84367677999994584</v>
       </c>
-      <c r="D21" s="1">
+      <c r="R21" s="1">
         <v>0.21640443999995185</v>
       </c>
-      <c r="E21" s="1">
-        <v>0.12300000000000111</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A22" s="5" t="s">
+      <c r="S21" s="1">
+        <v>0.12300000000000111</v>
+      </c>
+    </row>
+    <row r="22" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="O22" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="B22" s="1">
-        <v>0</v>
-      </c>
-      <c r="C22" s="1">
+      <c r="P22" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q22" s="1">
         <v>0.20492825999996711</v>
       </c>
-      <c r="D22" s="1">
+      <c r="R22" s="1">
         <v>3.1399299999964825E-2</v>
       </c>
-      <c r="E22" s="1">
-        <v>0.12300000000000111</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A23" s="5" t="s">
+      <c r="S22" s="1">
+        <v>0.12300000000000111</v>
+      </c>
+    </row>
+    <row r="23" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="O23" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B23" s="1">
-        <v>0</v>
-      </c>
-      <c r="C23" s="1">
+      <c r="P23" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q23" s="1">
         <v>0.50867605999996357</v>
       </c>
-      <c r="D23" s="1">
+      <c r="R23" s="1">
         <v>-0.14474954000003137</v>
       </c>
-      <c r="E23" s="1">
-        <v>0.12300000000000111</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A24" s="5" t="s">
+      <c r="S23" s="1">
+        <v>0.12300000000000111</v>
+      </c>
+    </row>
+    <row r="24" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="O24" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B24" s="1">
-        <v>0</v>
-      </c>
-      <c r="C24" s="1">
+      <c r="P24" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q24" s="1">
         <v>0.59255065000001395</v>
       </c>
-      <c r="D24" s="1">
+      <c r="R24" s="1">
         <v>-0.33148215000001002</v>
       </c>
-      <c r="E24" s="1">
-        <v>0.12300000000000111</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A25" s="1" t="s">
+      <c r="S24" s="1">
+        <v>0.12300000000000111</v>
+      </c>
+    </row>
+    <row r="25" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="O25" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B25" s="1">
-        <v>0</v>
-      </c>
-      <c r="C25" s="1">
+      <c r="P25" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q25" s="1">
         <v>0.50554635000002435</v>
       </c>
-      <c r="D25" s="1">
+      <c r="R25" s="1">
         <v>-0.6216317699999756</v>
       </c>
-      <c r="E25" s="1">
-        <v>0.12300000000000111</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A26" s="1" t="s">
+      <c r="S25" s="1">
+        <v>0.12300000000000111</v>
+      </c>
+    </row>
+    <row r="26" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="O26" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B26" s="1">
-        <v>0</v>
-      </c>
-      <c r="C26" s="1">
+      <c r="P26" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q26" s="1">
         <v>0.89115173999999087</v>
       </c>
-      <c r="D26" s="1">
+      <c r="R26" s="1">
         <v>-0.65971805999999944</v>
       </c>
-      <c r="E26" s="1">
-        <v>0.12300000000000111</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A27" s="1" t="s">
+      <c r="S26" s="1">
+        <v>0.12300000000000111</v>
+      </c>
+    </row>
+    <row r="27" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="O27" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B27" s="1">
-        <v>0</v>
-      </c>
-      <c r="C27" s="1">
+      <c r="P27" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q27" s="1">
         <v>0.62801460999997261</v>
       </c>
-      <c r="D27" s="1">
+      <c r="R27" s="1">
         <v>-0.52560204000003452</v>
       </c>
-      <c r="E27" s="1">
-        <v>0.12300000000000111</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A28" s="1" t="s">
+      <c r="S27" s="1">
+        <v>0.12300000000000111</v>
+      </c>
+    </row>
+    <row r="28" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="O28" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B28" s="1">
-        <v>0</v>
-      </c>
-      <c r="C28" s="1">
+      <c r="P28" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q28" s="1">
         <v>1.0472342099999921</v>
       </c>
-      <c r="D28" s="1">
+      <c r="R28" s="1">
         <v>3.4994419999964776E-2</v>
       </c>
-      <c r="E28" s="1">
-        <v>0.12300000000000111</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A29" s="1" t="s">
+      <c r="S28" s="1">
+        <v>0.12300000000000111</v>
+      </c>
+    </row>
+    <row r="29" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="O29" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B29" s="1">
-        <v>0</v>
-      </c>
-      <c r="C29" s="1">
+      <c r="P29" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q29" s="1">
         <v>1.6170278100000175</v>
       </c>
-      <c r="D29" s="1">
+      <c r="R29" s="1">
         <v>0.37293717999999743</v>
       </c>
-      <c r="E29" s="1">
-        <v>0.12300000000000111</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A30" s="5" t="s">
+      <c r="S29" s="1">
+        <v>0.12300000000000111</v>
+      </c>
+    </row>
+    <row r="30" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="O30" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="B30" s="1">
-        <v>0</v>
-      </c>
-      <c r="C30" s="1">
+      <c r="P30" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q30" s="1">
         <v>0.86854102000000211</v>
       </c>
-      <c r="D30" s="1">
+      <c r="R30" s="1">
         <v>0.45489865999995871</v>
       </c>
-      <c r="E30" s="1">
-        <v>0.12300000000000111</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A31" s="5" t="s">
+      <c r="S30" s="1">
+        <v>0.12300000000000111</v>
+      </c>
+    </row>
+    <row r="31" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="O31" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="B31" s="1">
-        <v>0</v>
-      </c>
-      <c r="C31" s="1">
+      <c r="P31" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q31" s="1">
         <v>-0.18472628000001379</v>
       </c>
-      <c r="D31" s="1">
+      <c r="R31" s="1">
         <v>4.0702499999731856E-3</v>
       </c>
-      <c r="E31" s="1">
-        <v>0.12300000000000111</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A32" s="5" t="s">
+      <c r="S31" s="1">
+        <v>0.12300000000000111</v>
+      </c>
+    </row>
+    <row r="32" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="O32" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="B32" s="1">
-        <v>0</v>
-      </c>
-      <c r="C32" s="1">
+      <c r="P32" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q32" s="1">
         <v>0.4962419299999894</v>
       </c>
-      <c r="D32" s="1">
+      <c r="R32" s="1">
         <v>-0.12233271999998507</v>
       </c>
-      <c r="E32" s="1">
-        <v>0.12300000000000111</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A33" s="5" t="s">
+      <c r="S32" s="1">
+        <v>0.12300000000000111</v>
+      </c>
+    </row>
+    <row r="33" spans="15:19" x14ac:dyDescent="0.35">
+      <c r="O33" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="B33" s="1">
-        <v>0</v>
-      </c>
-      <c r="C33" s="1">
+      <c r="P33" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q33" s="1">
         <v>0.54488558999997139</v>
       </c>
-      <c r="D33" s="1">
+      <c r="R33" s="1">
         <v>-0.19933409999999796</v>
       </c>
-      <c r="E33" s="1">
-        <v>0.12300000000000111</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A34" s="1" t="s">
+      <c r="S33" s="1">
+        <v>0.12300000000000111</v>
+      </c>
+    </row>
+    <row r="34" spans="15:19" x14ac:dyDescent="0.35">
+      <c r="O34" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B34" s="1">
-        <v>0</v>
-      </c>
-      <c r="C34" s="1">
+      <c r="P34" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q34" s="1">
         <v>0.33292057999999969</v>
       </c>
-      <c r="D34" s="1">
+      <c r="R34" s="1">
         <v>-0.48480682000002773</v>
       </c>
-      <c r="E34" s="1">
-        <v>0.12300000000000111</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A35" s="1" t="s">
+      <c r="S34" s="1">
+        <v>0.12300000000000111</v>
+      </c>
+    </row>
+    <row r="35" spans="15:19" x14ac:dyDescent="0.35">
+      <c r="O35" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B35" s="1">
-        <v>0</v>
-      </c>
-      <c r="C35" s="1">
+      <c r="P35" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q35" s="1">
         <v>0.71068052999998343</v>
       </c>
-      <c r="D35" s="1">
+      <c r="R35" s="1">
         <v>-0.7608479800000616</v>
       </c>
-      <c r="E35" s="1">
-        <v>0.12300000000000111</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A36" s="1" t="s">
+      <c r="S35" s="1">
+        <v>0.12300000000000111</v>
+      </c>
+    </row>
+    <row r="36" spans="15:19" x14ac:dyDescent="0.35">
+      <c r="O36" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B36" s="1">
-        <v>0</v>
-      </c>
-      <c r="C36" s="1">
+      <c r="P36" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q36" s="1">
         <v>0.90776295999994971</v>
       </c>
-      <c r="D36" s="1">
+      <c r="R36" s="1">
         <v>-0.15853684000002133</v>
       </c>
-      <c r="E36" s="1">
-        <v>0.12300000000000111</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A37" s="1" t="s">
+      <c r="S36" s="1">
+        <v>0.12300000000000111</v>
+      </c>
+    </row>
+    <row r="37" spans="15:19" x14ac:dyDescent="0.35">
+      <c r="O37" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B37" s="1">
-        <v>0</v>
-      </c>
-      <c r="C37" s="1">
+      <c r="P37" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q37" s="1">
         <v>1.9748885499999957</v>
       </c>
-      <c r="D37" s="1">
+      <c r="R37" s="1">
         <v>0.47546450000003304</v>
       </c>
-      <c r="E37" s="1">
+      <c r="S37" s="1">
         <v>0.12300000000000111</v>
       </c>
     </row>
@@ -3525,15 +4059,15 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E37"/>
+  <dimension ref="A1:S37"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23:E23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.35">
       <c r="B1" t="s">
         <v>24</v>
       </c>
@@ -3546,596 +4080,863 @@
       <c r="E1" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
+      <c r="P1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>1</v>
+      </c>
+      <c r="R1" t="s">
+        <v>2</v>
+      </c>
+      <c r="S1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B2">
-        <v>0</v>
-      </c>
-      <c r="C2">
+      <c r="B2" s="1">
+        <v>0</v>
+      </c>
+      <c r="C2" s="1">
         <v>0.84367677999994584</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="1">
         <v>0.21640443999995185</v>
       </c>
-      <c r="E2">
-        <v>0.12300000000000111</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
+      <c r="E2" s="1">
+        <v>0.12300000000000111</v>
+      </c>
+      <c r="O2" t="s">
+        <v>26</v>
+      </c>
+      <c r="P2">
+        <v>0</v>
+      </c>
+      <c r="Q2">
+        <v>0.84367677999994584</v>
+      </c>
+      <c r="R2">
+        <v>0.21640443999995185</v>
+      </c>
+      <c r="S2">
+        <v>0.12300000000000111</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A3" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="B3">
-        <v>0</v>
-      </c>
-      <c r="C3">
+      <c r="B3" s="1">
+        <v>0</v>
+      </c>
+      <c r="C3" s="1">
+        <v>-3.9294530400000056</v>
+      </c>
+      <c r="D3" s="1">
+        <v>-3.3327692599999743</v>
+      </c>
+      <c r="E3" s="1">
+        <v>0.12300000000000111</v>
+      </c>
+      <c r="O3" t="s">
+        <v>27</v>
+      </c>
+      <c r="P3">
+        <v>0</v>
+      </c>
+      <c r="Q3">
         <v>-3.9298673199999783</v>
       </c>
-      <c r="D3">
+      <c r="R3">
         <v>-3.3318463999999715</v>
       </c>
-      <c r="E3">
-        <v>0.12300000000000111</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
+      <c r="S3">
+        <v>0.12300000000000111</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A4" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B4">
-        <v>0</v>
-      </c>
-      <c r="C4">
+      <c r="B4" s="1">
+        <v>0</v>
+      </c>
+      <c r="C4" s="1">
         <v>0.77267884999996994</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="1">
         <v>-0.13173776000003201</v>
       </c>
-      <c r="E4">
-        <v>0.12300000000000111</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
+      <c r="E4" s="1">
+        <v>0.12300000000000111</v>
+      </c>
+      <c r="O4" t="s">
+        <v>12</v>
+      </c>
+      <c r="P4">
+        <v>0</v>
+      </c>
+      <c r="Q4">
+        <v>0.77267884999996994</v>
+      </c>
+      <c r="R4">
+        <v>-0.13173776000003201</v>
+      </c>
+      <c r="S4">
+        <v>0.12300000000000111</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A5" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B5">
-        <v>0</v>
-      </c>
-      <c r="C5">
+      <c r="B5" s="1">
+        <v>0</v>
+      </c>
+      <c r="C5" s="1">
         <v>0.5980749399999965</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="1">
+        <v>0.49119933000001836</v>
+      </c>
+      <c r="E5" s="1">
+        <v>0.12300000000000111</v>
+      </c>
+      <c r="O5" t="s">
+        <v>7</v>
+      </c>
+      <c r="P5">
+        <v>0</v>
+      </c>
+      <c r="Q5">
+        <v>0.5980749399999965</v>
+      </c>
+      <c r="R5">
         <v>-0.34750837000002477</v>
       </c>
-      <c r="E5">
-        <v>0.12300000000000111</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
+      <c r="S5">
+        <v>0.12300000000000111</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A6" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B6">
-        <v>0</v>
-      </c>
-      <c r="C6">
+      <c r="B6" s="1">
+        <v>0</v>
+      </c>
+      <c r="C6" s="1">
         <v>0.19830491999999111</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="1">
         <v>-1.0079512099999981</v>
       </c>
-      <c r="E6">
-        <v>0.12300000000000111</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
+      <c r="E6" s="1">
+        <v>0.12300000000000111</v>
+      </c>
+      <c r="O6" t="s">
+        <v>9</v>
+      </c>
+      <c r="P6">
+        <v>0</v>
+      </c>
+      <c r="Q6">
+        <v>0.19830491999999111</v>
+      </c>
+      <c r="R6">
+        <v>-1.0079512099999981</v>
+      </c>
+      <c r="S6">
+        <v>0.12300000000000111</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A7" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B7">
-        <v>0</v>
-      </c>
-      <c r="C7">
+      <c r="B7" s="1">
+        <v>0</v>
+      </c>
+      <c r="C7" s="1">
         <v>-1.1515078100000053</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="1">
         <v>-1.0597707199999711</v>
       </c>
-      <c r="E7">
-        <v>0.12300000000000111</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
+      <c r="E7" s="1">
+        <v>0.12300000000000111</v>
+      </c>
+      <c r="O7" t="s">
+        <v>10</v>
+      </c>
+      <c r="P7">
+        <v>0</v>
+      </c>
+      <c r="Q7">
+        <v>-1.1515078100000053</v>
+      </c>
+      <c r="R7">
+        <v>-1.0597707199999711</v>
+      </c>
+      <c r="S7">
+        <v>0.12300000000000111</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B8">
-        <v>0</v>
-      </c>
-      <c r="C8">
+      <c r="B8" s="1">
+        <v>0</v>
+      </c>
+      <c r="C8" s="1">
         <v>-0.31987263000002741</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="1">
         <v>-0.68671337000001742</v>
       </c>
-      <c r="E8">
-        <v>0.12300000000000111</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
+      <c r="E8" s="1">
+        <v>0.12300000000000111</v>
+      </c>
+      <c r="O8" t="s">
+        <v>6</v>
+      </c>
+      <c r="P8">
+        <v>0</v>
+      </c>
+      <c r="Q8">
+        <v>-0.31987263000002741</v>
+      </c>
+      <c r="R8">
+        <v>-0.68671337000001742</v>
+      </c>
+      <c r="S8">
+        <v>0.12300000000000111</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A9" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B9">
-        <v>0</v>
-      </c>
-      <c r="C9">
+      <c r="B9" s="1">
+        <v>0</v>
+      </c>
+      <c r="C9" s="1">
         <v>-2.4497010000011699E-2</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="1">
         <v>-0.42002953999998383</v>
       </c>
-      <c r="E9">
-        <v>0.12300000000000111</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
+      <c r="E9" s="1">
+        <v>0.12300000000000111</v>
+      </c>
+      <c r="O9" t="s">
+        <v>5</v>
+      </c>
+      <c r="P9">
+        <v>0</v>
+      </c>
+      <c r="Q9">
+        <v>-2.4497010000011699E-2</v>
+      </c>
+      <c r="R9">
+        <v>-0.42002953999998383</v>
+      </c>
+      <c r="S9">
+        <v>0.12300000000000111</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A10" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="B10">
-        <v>0</v>
-      </c>
-      <c r="C10">
+      <c r="B10" s="1">
+        <v>0</v>
+      </c>
+      <c r="C10" s="1">
+        <v>1.5144239500000296</v>
+      </c>
+      <c r="D10" s="1">
+        <v>0.39521928999998934</v>
+      </c>
+      <c r="E10" s="1">
+        <v>0.12300000000000111</v>
+      </c>
+      <c r="O10" t="s">
+        <v>28</v>
+      </c>
+      <c r="P10">
+        <v>0</v>
+      </c>
+      <c r="Q10">
         <v>1.388261419999985</v>
       </c>
-      <c r="D10">
+      <c r="R10">
         <v>0.24627239999999873</v>
       </c>
-      <c r="E10">
-        <v>0.12300000000000111</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
+      <c r="S10">
+        <v>0.12300000000000111</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A11" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="B11">
-        <v>0</v>
-      </c>
-      <c r="C11">
+      <c r="B11" s="1">
+        <v>0</v>
+      </c>
+      <c r="C11" s="1">
         <v>-1.4844687900000011</v>
       </c>
-      <c r="D11">
+      <c r="D11" s="1">
         <v>-2.3943126300000124</v>
       </c>
-      <c r="E11">
-        <v>0.12300000000000111</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
+      <c r="E11" s="1">
+        <v>0.12300000000000111</v>
+      </c>
+      <c r="O11" t="s">
+        <v>29</v>
+      </c>
+      <c r="P11">
+        <v>0</v>
+      </c>
+      <c r="Q11">
+        <v>-1.4844687900000011</v>
+      </c>
+      <c r="R11">
+        <v>-2.3943126300000124</v>
+      </c>
+      <c r="S11">
+        <v>0.12300000000000111</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A12" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="B12">
-        <v>0</v>
-      </c>
-      <c r="C12">
+      <c r="B12" s="1">
+        <v>0</v>
+      </c>
+      <c r="C12" s="1">
         <v>-15.760328099999988</v>
       </c>
-      <c r="D12">
+      <c r="D12" s="1">
+        <v>-9.7994835600000094</v>
+      </c>
+      <c r="E12" s="1">
+        <v>0.12300000000000111</v>
+      </c>
+      <c r="O12" t="s">
+        <v>30</v>
+      </c>
+      <c r="P12">
+        <v>0</v>
+      </c>
+      <c r="Q12">
+        <v>-15.760328099999988</v>
+      </c>
+      <c r="R12">
         <v>-9.2350458500000165</v>
       </c>
-      <c r="E12">
-        <v>0.12300000000000111</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
+      <c r="S12">
+        <v>0.12300000000000111</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A13" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="B13">
-        <v>0</v>
-      </c>
-      <c r="C13">
+      <c r="B13" s="1">
+        <v>0</v>
+      </c>
+      <c r="C13" s="1">
+        <v>-0.33259743000002828</v>
+      </c>
+      <c r="D13" s="1">
+        <v>-0.16926831000001741</v>
+      </c>
+      <c r="E13" s="1">
+        <v>0.12300000000000111</v>
+      </c>
+      <c r="O13" t="s">
+        <v>31</v>
+      </c>
+      <c r="P13">
+        <v>0</v>
+      </c>
+      <c r="Q13">
         <v>-0.83848961000001765</v>
       </c>
-      <c r="D13">
+      <c r="R13">
         <v>-0.16965888000005336</v>
       </c>
-      <c r="E13">
-        <v>0.12300000000000111</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
+      <c r="S13">
+        <v>0.12300000000000111</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A14" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="B14">
-        <v>0</v>
-      </c>
-      <c r="C14">
+      <c r="B14" s="1">
+        <v>0</v>
+      </c>
+      <c r="C14" s="1">
         <v>0.93347217000000882</v>
       </c>
-      <c r="D14">
+      <c r="D14" s="1">
+        <v>0.48638604000000285</v>
+      </c>
+      <c r="E14" s="1">
+        <v>0.12300000000000111</v>
+      </c>
+      <c r="O14" t="s">
+        <v>32</v>
+      </c>
+      <c r="P14">
+        <v>0</v>
+      </c>
+      <c r="Q14">
+        <v>0.93347217000000882</v>
+      </c>
+      <c r="R14">
         <v>-0.10062783999996938</v>
       </c>
-      <c r="E14">
-        <v>0.12300000000000111</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A15" t="s">
+      <c r="S14">
+        <v>0.12300000000000111</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A15" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B15">
-        <v>0</v>
-      </c>
-      <c r="C15">
+      <c r="B15" s="1">
+        <v>0</v>
+      </c>
+      <c r="C15" s="1">
         <v>0.71765909999998456</v>
       </c>
-      <c r="D15">
+      <c r="D15" s="1">
         <v>-0.57658672999998473</v>
       </c>
-      <c r="E15">
-        <v>0.12300000000000111</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A16" t="s">
+      <c r="E15" s="1">
+        <v>0.12300000000000111</v>
+      </c>
+      <c r="O15" t="s">
+        <v>33</v>
+      </c>
+      <c r="P15">
+        <v>0</v>
+      </c>
+      <c r="Q15">
+        <v>0.71765909999998456</v>
+      </c>
+      <c r="R15">
+        <v>-0.57658672999998473</v>
+      </c>
+      <c r="S15">
+        <v>0.12300000000000111</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A16" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B16">
-        <v>0</v>
-      </c>
-      <c r="C16">
+      <c r="B16" s="1">
+        <v>0</v>
+      </c>
+      <c r="C16" s="1">
         <v>0.38622984999999943</v>
       </c>
-      <c r="D16">
+      <c r="D16" s="1">
         <v>-1.0515337499999866</v>
       </c>
-      <c r="E16">
-        <v>0.12300000000000111</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A17" t="s">
+      <c r="E16" s="1">
+        <v>0.12300000000000111</v>
+      </c>
+      <c r="O16" t="s">
+        <v>34</v>
+      </c>
+      <c r="P16">
+        <v>0</v>
+      </c>
+      <c r="Q16">
+        <v>0.38622984999999943</v>
+      </c>
+      <c r="R16">
+        <v>-1.0515337499999866</v>
+      </c>
+      <c r="S16">
+        <v>0.12300000000000111</v>
+      </c>
+    </row>
+    <row r="17" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A17" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B17">
-        <v>0</v>
-      </c>
-      <c r="C17">
+      <c r="B17" s="1">
+        <v>0</v>
+      </c>
+      <c r="C17" s="1">
         <v>0.72695723999998307</v>
       </c>
-      <c r="D17">
+      <c r="D17" s="1">
         <v>-0.23061289999999346</v>
       </c>
-      <c r="E17">
-        <v>0.12300000000000111</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A18" t="s">
+      <c r="E17" s="1">
+        <v>0.12300000000000111</v>
+      </c>
+      <c r="O17" t="s">
+        <v>35</v>
+      </c>
+      <c r="P17">
+        <v>0</v>
+      </c>
+      <c r="Q17">
+        <v>0.72695723999998307</v>
+      </c>
+      <c r="R17">
+        <v>-0.23061289999999346</v>
+      </c>
+      <c r="S17">
+        <v>0.12300000000000111</v>
+      </c>
+    </row>
+    <row r="18" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A18" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="B18">
-        <v>0</v>
-      </c>
-      <c r="C18">
+      <c r="B18" s="1">
+        <v>0</v>
+      </c>
+      <c r="C18" s="1">
+        <v>1.777038769999983</v>
+      </c>
+      <c r="D18" s="1">
+        <v>0.27110600999997203</v>
+      </c>
+      <c r="E18" s="1">
+        <v>0.12300000000000111</v>
+      </c>
+      <c r="O18" t="s">
+        <v>36</v>
+      </c>
+      <c r="P18">
+        <v>0</v>
+      </c>
+      <c r="Q18">
         <v>-0.64612740000001878</v>
       </c>
-      <c r="D18">
+      <c r="R18">
         <v>0.36059721999997763</v>
       </c>
-      <c r="E18">
-        <v>0.12300000000000111</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B20" t="s">
+      <c r="S18">
+        <v>0.12300000000000111</v>
+      </c>
+    </row>
+    <row r="20" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="P20" t="s">
         <v>24</v>
       </c>
-      <c r="C20" t="s">
+      <c r="Q20" t="s">
         <v>1</v>
       </c>
-      <c r="D20" t="s">
+      <c r="R20" t="s">
         <v>2</v>
       </c>
-      <c r="E20" t="s">
+      <c r="S20" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A21" s="1" t="s">
+    <row r="21" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="O21" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B21" s="1">
-        <v>0</v>
-      </c>
-      <c r="C21" s="1">
+      <c r="P21" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q21" s="1">
         <v>0.84367677999994584</v>
       </c>
-      <c r="D21" s="1">
+      <c r="R21" s="1">
         <v>0.21640443999995185</v>
       </c>
-      <c r="E21" s="1">
-        <v>0.12300000000000111</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A22" s="5" t="s">
+      <c r="S21" s="1">
+        <v>0.12300000000000111</v>
+      </c>
+    </row>
+    <row r="22" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="O22" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="B22" s="1">
-        <v>0</v>
-      </c>
-      <c r="C22" s="1">
+      <c r="P22" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q22" s="1">
         <v>-3.9294530400000056</v>
       </c>
-      <c r="D22" s="1">
+      <c r="R22" s="1">
         <v>-3.3327692599999743</v>
       </c>
-      <c r="E22" s="1">
-        <v>0.12300000000000111</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A23" s="1" t="s">
+      <c r="S22" s="1">
+        <v>0.12300000000000111</v>
+      </c>
+    </row>
+    <row r="23" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="O23" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B23" s="1">
-        <v>0</v>
-      </c>
-      <c r="C23" s="1">
+      <c r="P23" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q23" s="1">
         <v>0.77267884999996994</v>
       </c>
-      <c r="D23" s="1">
+      <c r="R23" s="1">
         <v>-0.13173776000003201</v>
       </c>
-      <c r="E23" s="1">
-        <v>0.12300000000000111</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A24" s="5" t="s">
+      <c r="S23" s="1">
+        <v>0.12300000000000111</v>
+      </c>
+    </row>
+    <row r="24" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="O24" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B24" s="1">
-        <v>0</v>
-      </c>
-      <c r="C24" s="1">
+      <c r="P24" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q24" s="1">
         <v>0.5980749399999965</v>
       </c>
-      <c r="D24" s="1">
+      <c r="R24" s="1">
         <v>0.49119933000001836</v>
       </c>
-      <c r="E24" s="1">
-        <v>0.12300000000000111</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A25" s="1" t="s">
+      <c r="S24" s="1">
+        <v>0.12300000000000111</v>
+      </c>
+    </row>
+    <row r="25" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="O25" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B25" s="1">
-        <v>0</v>
-      </c>
-      <c r="C25" s="1">
+      <c r="P25" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q25" s="1">
         <v>0.19830491999999111</v>
       </c>
-      <c r="D25" s="1">
+      <c r="R25" s="1">
         <v>-1.0079512099999981</v>
       </c>
-      <c r="E25" s="1">
-        <v>0.12300000000000111</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A26" s="1" t="s">
+      <c r="S25" s="1">
+        <v>0.12300000000000111</v>
+      </c>
+    </row>
+    <row r="26" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="O26" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B26" s="1">
-        <v>0</v>
-      </c>
-      <c r="C26" s="1">
+      <c r="P26" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q26" s="1">
         <v>-1.1515078100000053</v>
       </c>
-      <c r="D26" s="1">
+      <c r="R26" s="1">
         <v>-1.0597707199999711</v>
       </c>
-      <c r="E26" s="1">
-        <v>0.12300000000000111</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A27" s="1" t="s">
+      <c r="S26" s="1">
+        <v>0.12300000000000111</v>
+      </c>
+    </row>
+    <row r="27" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="O27" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B27" s="1">
-        <v>0</v>
-      </c>
-      <c r="C27" s="1">
+      <c r="P27" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q27" s="1">
         <v>-0.31987263000002741</v>
       </c>
-      <c r="D27" s="1">
+      <c r="R27" s="1">
         <v>-0.68671337000001742</v>
       </c>
-      <c r="E27" s="1">
-        <v>0.12300000000000111</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A28" s="1" t="s">
+      <c r="S27" s="1">
+        <v>0.12300000000000111</v>
+      </c>
+    </row>
+    <row r="28" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="O28" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B28" s="1">
-        <v>0</v>
-      </c>
-      <c r="C28" s="1">
+      <c r="P28" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q28" s="1">
         <v>-2.4497010000011699E-2</v>
       </c>
-      <c r="D28" s="1">
+      <c r="R28" s="1">
         <v>-0.42002953999998383</v>
       </c>
-      <c r="E28" s="1">
-        <v>0.12300000000000111</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A29" s="5" t="s">
+      <c r="S28" s="1">
+        <v>0.12300000000000111</v>
+      </c>
+    </row>
+    <row r="29" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="O29" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="B29" s="1">
-        <v>0</v>
-      </c>
-      <c r="C29" s="1">
+      <c r="P29" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q29" s="1">
         <v>1.5144239500000296</v>
       </c>
-      <c r="D29" s="1">
+      <c r="R29" s="1">
         <v>0.39521928999998934</v>
       </c>
-      <c r="E29" s="1">
-        <v>0.12300000000000111</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A30" s="5" t="s">
+      <c r="S29" s="1">
+        <v>0.12300000000000111</v>
+      </c>
+    </row>
+    <row r="30" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="O30" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="B30" s="1">
-        <v>0</v>
-      </c>
-      <c r="C30" s="1">
+      <c r="P30" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q30" s="1">
         <v>-1.4844687900000011</v>
       </c>
-      <c r="D30" s="1">
+      <c r="R30" s="1">
         <v>-2.3943126300000124</v>
       </c>
-      <c r="E30" s="1">
-        <v>0.12300000000000111</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A31" s="5" t="s">
+      <c r="S30" s="1">
+        <v>0.12300000000000111</v>
+      </c>
+    </row>
+    <row r="31" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="O31" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="B31" s="1">
-        <v>0</v>
-      </c>
-      <c r="C31" s="1">
+      <c r="P31" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q31" s="1">
         <v>-15.760328099999988</v>
       </c>
-      <c r="D31" s="1">
+      <c r="R31" s="1">
         <v>-9.7994835600000094</v>
       </c>
-      <c r="E31" s="1">
-        <v>0.12300000000000111</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A32" s="5" t="s">
+      <c r="S31" s="1">
+        <v>0.12300000000000111</v>
+      </c>
+    </row>
+    <row r="32" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="O32" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="B32" s="1">
-        <v>0</v>
-      </c>
-      <c r="C32" s="1">
+      <c r="P32" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q32" s="1">
         <v>-0.33259743000002828</v>
       </c>
-      <c r="D32" s="1">
+      <c r="R32" s="1">
         <v>-0.16926831000001741</v>
       </c>
-      <c r="E32" s="1">
-        <v>0.12300000000000111</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A33" s="5" t="s">
+      <c r="S32" s="1">
+        <v>0.12300000000000111</v>
+      </c>
+    </row>
+    <row r="33" spans="15:19" x14ac:dyDescent="0.35">
+      <c r="O33" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="B33" s="1">
-        <v>0</v>
-      </c>
-      <c r="C33" s="1">
+      <c r="P33" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q33" s="1">
         <v>0.93347217000000882</v>
       </c>
-      <c r="D33" s="1">
+      <c r="R33" s="1">
         <v>0.48638604000000285</v>
       </c>
-      <c r="E33" s="1">
-        <v>0.12300000000000111</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A34" s="1" t="s">
+      <c r="S33" s="1">
+        <v>0.12300000000000111</v>
+      </c>
+    </row>
+    <row r="34" spans="15:19" x14ac:dyDescent="0.35">
+      <c r="O34" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B34" s="1">
-        <v>0</v>
-      </c>
-      <c r="C34" s="1">
+      <c r="P34" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q34" s="1">
         <v>0.71765909999998456</v>
       </c>
-      <c r="D34" s="1">
+      <c r="R34" s="1">
         <v>-0.57658672999998473</v>
       </c>
-      <c r="E34" s="1">
-        <v>0.12300000000000111</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A35" s="1" t="s">
+      <c r="S34" s="1">
+        <v>0.12300000000000111</v>
+      </c>
+    </row>
+    <row r="35" spans="15:19" x14ac:dyDescent="0.35">
+      <c r="O35" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B35" s="1">
-        <v>0</v>
-      </c>
-      <c r="C35" s="1">
+      <c r="P35" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q35" s="1">
         <v>0.38622984999999943</v>
       </c>
-      <c r="D35" s="1">
+      <c r="R35" s="1">
         <v>-1.0515337499999866</v>
       </c>
-      <c r="E35" s="1">
-        <v>0.12300000000000111</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A36" s="1" t="s">
+      <c r="S35" s="1">
+        <v>0.12300000000000111</v>
+      </c>
+    </row>
+    <row r="36" spans="15:19" x14ac:dyDescent="0.35">
+      <c r="O36" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B36" s="1">
-        <v>0</v>
-      </c>
-      <c r="C36" s="1">
+      <c r="P36" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q36" s="1">
         <v>0.72695723999998307</v>
       </c>
-      <c r="D36" s="1">
+      <c r="R36" s="1">
         <v>-0.23061289999999346</v>
       </c>
-      <c r="E36" s="1">
-        <v>0.12300000000000111</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A37" s="5" t="s">
+      <c r="S36" s="1">
+        <v>0.12300000000000111</v>
+      </c>
+    </row>
+    <row r="37" spans="15:19" x14ac:dyDescent="0.35">
+      <c r="O37" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="B37" s="1">
-        <v>0</v>
-      </c>
-      <c r="C37" s="1">
+      <c r="P37" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q37" s="1">
         <v>1.777038769999983</v>
       </c>
-      <c r="D37" s="1">
+      <c r="R37" s="1">
         <v>0.27110600999997203</v>
       </c>
-      <c r="E37" s="1">
+      <c r="S37" s="1">
         <v>0.12300000000000111</v>
       </c>
     </row>

</xml_diff>